<commit_message>
Modif url canonique termino df9498eb894642b7264f6d5c9a38a249f1b02b34
</commit_message>
<xml_diff>
--- a/poc-professionnel/ig/StructureDefinition-Adresse.xlsx
+++ b/poc-professionnel/ig/StructureDefinition-Adresse.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-24T13:17:05+00:00</t>
+    <t>2025-07-25T07:22:51+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -300,7 +300,7 @@
     <t>preferred</t>
   </si>
   <si>
-    <t>https://interop.esante.gouv.fr/terminologies/CodeSystem-TRE-R35-TypeVoie?vs</t>
+    <t>https://mos.esante.gouv.fr/NOS/TRE_R35-TypeVoie/FHIR/TRE-R35-TypeVoie?vs</t>
   </si>
   <si>
     <t>Adresse.libelleVoie</t>
@@ -339,7 +339,7 @@
     <t>Code officiel géographique (COG), diffusé par l'INSEE, de la commune d'implantation du destinataire. Ce code ne fait pas partie de la norme NF Z 10-011 mais il correspond au libellé de l'attribut "localite" de la classe Adresse qui lui fait partie de la norme.</t>
   </si>
   <si>
-    <t>https://interop.esante.gouv.fr/terminologies/CodeSystem-TRE-R13-CommuneOM?vs</t>
+    <t>https://mos.esante.gouv.fr/NOS/TRE_R13-CommuneOM/FHIR/TRE-R13-CommuneOM?vs</t>
   </si>
   <si>
     <t>Adresse.internationalDivisionTerritoriale</t>
@@ -736,7 +736,7 @@
     <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="18.49609375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="66.875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="69.6171875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="17.65625" customWidth="true" bestFit="true"/>

</xml_diff>